<commit_message>
fixed categories, associations, cleared rubocop errors, added categories
</commit_message>
<xml_diff>
--- a/droidstore/checklist.xlsx
+++ b/droidstore/checklist.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="87">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="87">
   <si>
     <t>admin dashboard</t>
   </si>
@@ -617,15 +617,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:F41"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="D42" sqref="D42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="9.140625" style="2"/>
     <col min="3" max="3" width="16.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="30.85546875" customWidth="1"/>
+    <col min="4" max="4" width="104" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:6" x14ac:dyDescent="0.25">
@@ -680,17 +680,20 @@
       </c>
     </row>
     <row r="4" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B4" s="2">
+      <c r="B4" s="3">
         <v>1.3</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C4" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="D4" t="s">
-        <v>5</v>
-      </c>
-      <c r="E4">
-        <v>2</v>
+      <c r="D4" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="E4" s="1">
+        <v>2</v>
+      </c>
+      <c r="F4" t="s">
+        <v>85</v>
       </c>
     </row>
     <row r="5" spans="2:6" x14ac:dyDescent="0.25">
@@ -708,17 +711,20 @@
       </c>
     </row>
     <row r="6" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B6" s="2">
+      <c r="B6" s="3">
         <v>1.5</v>
       </c>
-      <c r="C6" t="s">
+      <c r="C6" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="D6" t="s">
+      <c r="D6" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="E6">
-        <v>5</v>
+      <c r="E6" s="1">
+        <v>5</v>
+      </c>
+      <c r="F6" t="s">
+        <v>85</v>
       </c>
     </row>
     <row r="7" spans="2:6" x14ac:dyDescent="0.25">
@@ -864,7 +870,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="17" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B17" s="2" t="s">
         <v>27</v>
       </c>
@@ -878,7 +884,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="18" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B18" s="2" t="s">
         <v>29</v>
       </c>
@@ -892,7 +898,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="19" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B19" s="2" t="s">
         <v>30</v>
       </c>
@@ -906,7 +912,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="20" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B20" s="2" t="s">
         <v>34</v>
       </c>
@@ -920,7 +926,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="21" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B21" s="2" t="s">
         <v>44</v>
       </c>
@@ -934,7 +940,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="22" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B22" s="2" t="s">
         <v>45</v>
       </c>
@@ -948,7 +954,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="23" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B23" s="2" t="s">
         <v>46</v>
       </c>
@@ -962,7 +968,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="24" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B24" s="2" t="s">
         <v>47</v>
       </c>
@@ -976,7 +982,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="25" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B25" s="2" t="s">
         <v>48</v>
       </c>
@@ -990,7 +996,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="26" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B26" s="2" t="s">
         <v>49</v>
       </c>
@@ -1004,7 +1010,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="27" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B27" s="2" t="s">
         <v>50</v>
       </c>
@@ -1018,35 +1024,41 @@
         <v>2</v>
       </c>
     </row>
-    <row r="28" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B28" s="2" t="s">
+    <row r="28" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B28" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="C28" t="s">
+      <c r="C28" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="D28" t="s">
+      <c r="D28" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="E28">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="29" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B29" s="2" t="s">
+      <c r="E28" s="1">
+        <v>2</v>
+      </c>
+      <c r="F28" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="29" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B29" s="3" t="s">
         <v>59</v>
       </c>
-      <c r="C29" t="s">
+      <c r="C29" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="D29" t="s">
+      <c r="D29" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="E29">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="30" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="E29" s="1">
+        <v>2</v>
+      </c>
+      <c r="F29" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="30" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B30" s="2" t="s">
         <v>60</v>
       </c>
@@ -1060,7 +1072,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="31" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="31" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B31" s="2" t="s">
         <v>61</v>
       </c>
@@ -1074,7 +1086,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="32" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="32" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B32" s="2" t="s">
         <v>62</v>
       </c>
@@ -1106,17 +1118,20 @@
       </c>
     </row>
     <row r="34" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B34" s="2" t="s">
+      <c r="B34" s="3" t="s">
         <v>73</v>
       </c>
-      <c r="C34" t="s">
+      <c r="C34" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="D34" t="s">
+      <c r="D34" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="E34">
-        <v>5</v>
+      <c r="E34" s="1">
+        <v>5</v>
+      </c>
+      <c r="F34" t="s">
+        <v>85</v>
       </c>
     </row>
     <row r="35" spans="2:6" x14ac:dyDescent="0.25">

</xml_diff>